<commit_message>
- added test cases for ordering products
</commit_message>
<xml_diff>
--- a/Burgerama Burger Shop App/material/TestCases.xlsx
+++ b/Burgerama Burger Shop App/material/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanoll\source\repos\burgerama-burger-shop\Burgerama Burger Shop App\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1002D6-7C35-41EA-94FD-819E2EF40298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABA38D6-A0D8-4033-B6EB-16561446441F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-6105" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,9 @@
   <si>
     <t>1) Enter either "1" or "2" in the Menu
 2) Press Enter</t>
+  </si>
+  <si>
+    <t>UI012</t>
   </si>
   <si>
     <t>UI001-N</t>
@@ -246,6 +249,235 @@
   <si>
     <t>Registration will be continued.
 The User will be promted to enter a city</t>
+  </si>
+  <si>
+    <t>UI006-N</t>
+  </si>
+  <si>
+    <t>The Registration asks for a city. The Input cant be empty and muts be a german city for delivery purpouses</t>
+  </si>
+  <si>
+    <t>During Registration a valid Email,Password,Street and ZIP have to be entered</t>
+  </si>
+  <si>
+    <t>The Input won`t be accepted and the User will be promted to enter a valid city</t>
+  </si>
+  <si>
+    <t>UI006-P</t>
+  </si>
+  <si>
+    <t>1) Enter: Tuttlingen
+2) Press Enter
+3) Press Enter</t>
+  </si>
+  <si>
+    <t>Registration is completed and the User should be back at the main menu</t>
+  </si>
+  <si>
+    <t>UI007-N</t>
+  </si>
+  <si>
+    <t>The User will be promted to LogIn using a registered Email</t>
+  </si>
+  <si>
+    <t>Login is chosen from the main menu</t>
+  </si>
+  <si>
+    <t>The Input wont be accepted an the
+User should be promted to use a valid and taken Email</t>
+  </si>
+  <si>
+    <t>UI007-P</t>
+  </si>
+  <si>
+    <t>The Input will be accepted and the User will be promted to enter a password</t>
+  </si>
+  <si>
+    <t>UI008-N</t>
+  </si>
+  <si>
+    <t>The User will be promted to LogIn using a password connected to a registered Email</t>
+  </si>
+  <si>
+    <t>Login is chosen from the main menu and a registered email was entered</t>
+  </si>
+  <si>
+    <t>Input: Literally anything different than the correct password</t>
+  </si>
+  <si>
+    <t>UI008-P</t>
+  </si>
+  <si>
+    <t>UI009-N</t>
+  </si>
+  <si>
+    <t>The User can order a Product by using the number on the most left side of the table</t>
+  </si>
+  <si>
+    <t>The User is successfully logged in after choosing login from the main menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Input must be invisible during the whole Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The Login information will be accepted, the user will be logged in and redirected to the ordermenu where a list of products should appear with the useres email at the top</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Input must be invisible during the whole Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The User will be told that the login credentials were incorrect and has to enter the email and password again</t>
+    </r>
+  </si>
+  <si>
+    <t>Input: - numbers outside of "1" and "14", 
+- negative numbers,
+- words and characters</t>
+  </si>
+  <si>
+    <t>The Input wont be accepted an the
+User should be promted to enter a valid option</t>
+  </si>
+  <si>
+    <t>UI009-P</t>
+  </si>
+  <si>
+    <t>1) Enter: 1
+2) Press Enter</t>
+  </si>
+  <si>
+    <t>UI010-N</t>
+  </si>
+  <si>
+    <t>The User can order a Product by using the number on the most left side of the table. We are ordering  a Drink which has the option to get it with or without ice</t>
+  </si>
+  <si>
+    <t>Input: - nothing
+- just spaces
+- words or characters
+- negative and positive numbers</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Press: 7 and the Press Enter
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repeat for every given Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Enter anything from the Input
+2) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <t>The Application should ask if the user wants his drink with or without Ice. But we are not entering true or false so the User will be promted to make a valid input. The Product will not be put into the shopping cart.</t>
+  </si>
+  <si>
+    <t>UI010-P</t>
+  </si>
+  <si>
+    <t>Input: - true
+              - false</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repeat for every given Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Press: 7
+2) Press Enter
+3) Enter: [Input]
+4) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <t>The Input should be accepted and behind the Price of the Coca Cola a (1) should appear</t>
+  </si>
+  <si>
+    <t>The Input should be accepted and behind the Price of the Cheeseburger a (1) should appear</t>
+  </si>
+  <si>
+    <t>UI011-N</t>
+  </si>
+  <si>
+    <t>The User can order a Product by using the number on the most left side of the table. We are ordering  a Hoodie which has the option to choose a size</t>
+  </si>
+  <si>
+    <t>UI011-P</t>
+  </si>
+  <si>
+    <t>We choose a few products and now want to finish our order, want to see what we ordered, where it is delivered to, how much it costs and how long it will take</t>
+  </si>
+  <si>
+    <t>The User has put the previously given products into his shopping cart</t>
   </si>
 </sst>
 </file>
@@ -275,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +517,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +566,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -343,6 +584,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1849755</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>426721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4402834</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>2952751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C3EE32C-AA87-4416-8230-A58561524878}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect t="2107" r="4053" b="11769"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13279755" y="15142846"/>
+          <a:ext cx="2553079" cy="2526030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -610,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +910,7 @@
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="36.109375" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
     <col min="7" max="7" width="51" customWidth="1"/>
     <col min="8" max="8" width="69.5546875" customWidth="1"/>
     <col min="9" max="9" width="10.21875" customWidth="1"/>
@@ -651,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -662,19 +951,21 @@
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="2:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -682,310 +973,438 @@
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="2:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="2:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="5"/>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+    <row r="14" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+    <row r="15" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+    <row r="20" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="5"/>
+      <c r="C20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+    <row r="21" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="5"/>
+      <c r="C21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+    <row r="22" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+    <row r="23" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B23" s="5"/>
+      <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+    <row r="24" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="5"/>
+      <c r="C24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+    <row r="25" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
+      <c r="C25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+    <row r="26" spans="2:9" ht="240.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="5"/>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -2009,5 +2428,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- added test cases for UI
</commit_message>
<xml_diff>
--- a/Burgerama Burger Shop App/material/TestCases.xlsx
+++ b/Burgerama Burger Shop App/material/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanoll\source\repos\burgerama-burger-shop\Burgerama Burger Shop App\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABA38D6-A0D8-4033-B6EB-16561446441F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9853399-0889-4C46-9450-EB67BF7737A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-6105" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -57,10 +57,6 @@
     <t>The Application should redirect either to the Registration or the Login depending on the Input</t>
   </si>
   <si>
-    <t>1) Enter either "1" or "2" in the Menu
-2) Press Enter</t>
-  </si>
-  <si>
     <t>UI012</t>
   </si>
   <si>
@@ -83,11 +79,6 @@
   </si>
   <si>
     <t>UI002-N</t>
-  </si>
-  <si>
-    <t>Input: numbers other than "1" and "2", 
-negative numbers,
-words and characters</t>
   </si>
   <si>
     <r>
@@ -115,17 +106,7 @@
     </r>
   </si>
   <si>
-    <t>Input: - HelloFresh.de
-- different kinds of words
-- only positiv and negative numbers
-- taken email: Fabian.Noll@gmail.com</t>
-  </si>
-  <si>
     <t>User should be promted to use a valid or not taken Email</t>
-  </si>
-  <si>
-    <t>1) Enter: UserTest@ks.de
-2) Press Enter</t>
   </si>
   <si>
     <t>UI003-N</t>
@@ -151,15 +132,6 @@
   </si>
   <si>
     <t>During Registration a valid Email and Password have to be entered</t>
-  </si>
-  <si>
-    <t>Input: - nothing
-- one space</t>
-  </si>
-  <si>
-    <t>Input: - any given number
-- nothing
-- just spaces</t>
   </si>
   <si>
     <t>User will be prompted to enter a valid street</t>
@@ -210,14 +182,6 @@
     </r>
   </si>
   <si>
-    <t>1) Enter: testpassword
-2) Press Enter</t>
-  </si>
-  <si>
-    <t>1) Enter: Dr Karl Storz Straße 34
-2) Press Enter</t>
-  </si>
-  <si>
     <t>Registration will be continued.
 The User will be promted to enter a ZIP</t>
   </si>
@@ -231,102 +195,690 @@
     <t>During Registration a valid Email,Password and Street have to be entered</t>
   </si>
   <si>
-    <t>Input: - nothing
-- just spaces
+    <t>The Input won`t be accepted and the User will be promted to enter a valid ZIP-Code</t>
+  </si>
+  <si>
+    <t>UI005-P</t>
+  </si>
+  <si>
+    <t>Registration will be continued.
+The User will be promted to enter a city</t>
+  </si>
+  <si>
+    <t>UI006-N</t>
+  </si>
+  <si>
+    <t>The Registration asks for a city. The Input cant be empty and muts be a german city for delivery purpouses</t>
+  </si>
+  <si>
+    <t>During Registration a valid Email,Password,Street and ZIP have to be entered</t>
+  </si>
+  <si>
+    <t>The Input won`t be accepted and the User will be promted to enter a valid city</t>
+  </si>
+  <si>
+    <t>UI006-P</t>
+  </si>
+  <si>
+    <t>Registration is completed and the User should be back at the main menu</t>
+  </si>
+  <si>
+    <t>UI007-N</t>
+  </si>
+  <si>
+    <t>The User will be promted to LogIn using a registered Email</t>
+  </si>
+  <si>
+    <t>Login is chosen from the main menu</t>
+  </si>
+  <si>
+    <t>The Input wont be accepted an the
+User should be promted to use a valid and taken Email</t>
+  </si>
+  <si>
+    <t>UI007-P</t>
+  </si>
+  <si>
+    <t>The Input will be accepted and the User will be promted to enter a password</t>
+  </si>
+  <si>
+    <t>UI008-N</t>
+  </si>
+  <si>
+    <t>The User will be promted to LogIn using a password connected to a registered Email</t>
+  </si>
+  <si>
+    <t>Login is chosen from the main menu and a registered email was entered</t>
+  </si>
+  <si>
+    <t>Input: Literally anything different than the correct password</t>
+  </si>
+  <si>
+    <t>UI008-P</t>
+  </si>
+  <si>
+    <t>UI009-N</t>
+  </si>
+  <si>
+    <t>The User can order a Product by using the number on the most left side of the table</t>
+  </si>
+  <si>
+    <t>The User is successfully logged in after choosing login from the main menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Input must be invisible during the whole Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The Login information will be accepted, the user will be logged in and redirected to the ordermenu where a list of products should appear with the useres email at the top</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Input must be invisible during the whole Time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The User will be told that the login credentials were incorrect and has to enter the email and password again</t>
+    </r>
+  </si>
+  <si>
+    <t>The Input wont be accepted an the
+User should be promted to enter a valid option</t>
+  </si>
+  <si>
+    <t>UI009-P</t>
+  </si>
+  <si>
+    <t>UI010-N</t>
+  </si>
+  <si>
+    <t>The User can order a Product by using the number on the most left side of the table. We are ordering  a Drink which has the option to get it with or without ice</t>
+  </si>
+  <si>
+    <t>The Application should ask if the user wants his drink with or without Ice. But we are not entering true or false so the User will be promted to make a valid input. The Product will not be put into the shopping cart.</t>
+  </si>
+  <si>
+    <t>UI010-P</t>
+  </si>
+  <si>
+    <t>The Input should be accepted and behind the Price of the Coca Cola a (1) should appear</t>
+  </si>
+  <si>
+    <t>The Input should be accepted and behind the Price of the Cheeseburger a (1) should appear</t>
+  </si>
+  <si>
+    <t>UI011-N</t>
+  </si>
+  <si>
+    <t>The User can order a Product by using the number on the most left side of the table. We are ordering  a Hoodie which has the option to choose a size</t>
+  </si>
+  <si>
+    <t>UI011-P</t>
+  </si>
+  <si>
+    <t>We choose a few products and now want to finish our order, want to see what we ordered, where it is delivered to, how much it costs and how long it will take</t>
+  </si>
+  <si>
+    <t>The User has put the previously given products into his shopping cart</t>
+  </si>
+  <si>
+    <t>Input: - [true]
+              - [FALSE]</t>
+  </si>
+  <si>
+    <t>Input: - numbers outside of [1] and [14], 
+- negative numbers,
+- words and characters</t>
+  </si>
+  <si>
+    <t>[] = a variable that is to be put in exactly like given (without the Brackets of course) // [] means nothing // [ ] means just spaces</t>
+  </si>
+  <si>
+    <t>Input: [] ; [      ]</t>
+  </si>
+  <si>
+    <t>Input: - any given number
+- [] ; [   ]</t>
+  </si>
+  <si>
+    <t>Input: - [] ; [   ]
 - words or characters
 - negative numbers</t>
   </si>
   <si>
-    <t>The Input won`t be accepted and the User will be promted to enter a valid ZIP-Code</t>
-  </si>
-  <si>
-    <t>UI005-P</t>
-  </si>
-  <si>
-    <t>1) Enter: 78532
+    <t>Input: - [] ; [   ]
+- words or characters
+- negative and positive numbers</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Input: numbers other than </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+negative numbers,
+words and characters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Input: - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HelloFresh.de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- different kinds of words
+- only positiv and negative numbers
+- taken email: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fabian.Noll@gmail.com</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter either </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the Menu
 2) Press Enter</t>
-  </si>
-  <si>
-    <t>Registration will be continued.
-The User will be promted to enter a city</t>
-  </si>
-  <si>
-    <t>UI006-N</t>
-  </si>
-  <si>
-    <t>The Registration asks for a city. The Input cant be empty and muts be a german city for delivery purpouses</t>
-  </si>
-  <si>
-    <t>During Registration a valid Email,Password,Street and ZIP have to be entered</t>
-  </si>
-  <si>
-    <t>The Input won`t be accepted and the User will be promted to enter a valid city</t>
-  </si>
-  <si>
-    <t>UI006-P</t>
-  </si>
-  <si>
-    <t>1) Enter: Tuttlingen
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1) Enter:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserTest@ks.de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>testpassword</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1) Enter:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dr Karl Storz Straße 34</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>78532</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tuttlingen</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 2) Press Enter
 3) Press Enter</t>
-  </si>
-  <si>
-    <t>Registration is completed and the User should be back at the main menu</t>
-  </si>
-  <si>
-    <t>UI007-N</t>
-  </si>
-  <si>
-    <t>The User will be promted to LogIn using a registered Email</t>
-  </si>
-  <si>
-    <t>Login is chosen from the main menu</t>
-  </si>
-  <si>
-    <t>The Input wont be accepted an the
-User should be promted to use a valid and taken Email</t>
-  </si>
-  <si>
-    <t>UI007-P</t>
-  </si>
-  <si>
-    <t>The Input will be accepted and the User will be promted to enter a password</t>
-  </si>
-  <si>
-    <t>UI008-N</t>
-  </si>
-  <si>
-    <t>The User will be promted to LogIn using a password connected to a registered Email</t>
-  </si>
-  <si>
-    <t>Login is chosen from the main menu and a registered email was entered</t>
-  </si>
-  <si>
-    <t>Input: Literally anything different than the correct password</t>
-  </si>
-  <si>
-    <t>UI008-P</t>
-  </si>
-  <si>
-    <t>UI009-N</t>
-  </si>
-  <si>
-    <t>The User can order a Product by using the number on the most left side of the table</t>
-  </si>
-  <si>
-    <t>The User is successfully logged in after choosing login from the main menu</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Input must be invisible during the whole Time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserTest@ks.de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
     </r>
     <r>
       <rPr>
@@ -337,20 +889,44 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-The Login information will be accepted, the user will be logged in and redirected to the ordermenu where a list of products should appear with the useres email at the top</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Input must be invisible during the whole Time</t>
+2) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
     </r>
     <r>
       <rPr>
@@ -361,40 +937,123 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-The User will be told that the login credentials were incorrect and has to enter the email and password again</t>
-    </r>
-  </si>
-  <si>
-    <t>Input: - numbers outside of "1" and "14", 
-- negative numbers,
-- words and characters</t>
-  </si>
-  <si>
-    <t>The Input wont be accepted an the
-User should be promted to enter a valid option</t>
-  </si>
-  <si>
-    <t>UI009-P</t>
-  </si>
-  <si>
-    <t>1) Enter: 1
 2) Press Enter</t>
-  </si>
-  <si>
-    <t>UI010-N</t>
-  </si>
-  <si>
-    <t>The User can order a Product by using the number on the most left side of the table. We are ordering  a Drink which has the option to get it with or without ice</t>
-  </si>
-  <si>
-    <t>Input: - nothing
-- just spaces
-- words or characters
-- negative and positive numbers</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1) Press: 7 and the Press Enter
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repeat for every given Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2) Press Enter
+3) Enter from Input
+4) Press Enter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the Press Enter
 </t>
     </r>
     <r>
@@ -422,14 +1081,31 @@
     </r>
   </si>
   <si>
-    <t>The Application should ask if the user wants his drink with or without Ice. But we are not entering true or false so the User will be promted to make a valid input. The Product will not be put into the shopping cart.</t>
-  </si>
-  <si>
-    <t>UI010-P</t>
-  </si>
-  <si>
-    <t>Input: - true
-              - false</t>
+    <t>1) Enter: [14]
+2) Press Enter</t>
+  </si>
+  <si>
+    <t>The following Overview should come up and look like this:
+After Pressing Enter again the User should be linked back to the main menu</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Input: - [] ; [   ]
+- words or characters
+- negative and positive numbers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>except one of the sizes!</t>
+    </r>
   </si>
   <si>
     <r>
@@ -452,32 +1128,115 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-1) Press: 7
+1) Enter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[11]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 2) Press Enter
-3) Enter: [Input]
+3) Enter from Input
 4) Press Enter</t>
     </r>
   </si>
   <si>
-    <t>The Input should be accepted and behind the Price of the Coca Cola a (1) should appear</t>
-  </si>
-  <si>
-    <t>The Input should be accepted and behind the Price of the Cheeseburger a (1) should appear</t>
-  </si>
-  <si>
-    <t>UI011-N</t>
-  </si>
-  <si>
-    <t>The User can order a Product by using the number on the most left side of the table. We are ordering  a Hoodie which has the option to choose a size</t>
-  </si>
-  <si>
-    <t>UI011-P</t>
-  </si>
-  <si>
-    <t>We choose a few products and now want to finish our order, want to see what we ordered, where it is delivered to, how much it costs and how long it will take</t>
-  </si>
-  <si>
-    <t>The User has put the previously given products into his shopping cart</t>
+    <t>The Application should ask the user in which size they want their Hoodie. Nothing else except the size should be accepted as the input and the user should be promted to enter a valid size.</t>
+  </si>
+  <si>
+    <t>Allowed Input should be Uppercase as well as lowercase. We want an S,L and XXL</t>
+  </si>
+  <si>
+    <t>The Application should ask the user in which size they want their Hoodie. The Inout should be accepted and the Hoodie in its chosen size should be put in the shoppincart. The User should now have to possibility to order something else</t>
+  </si>
+  <si>
+    <t>UI013</t>
+  </si>
+  <si>
+    <t>We are not the User anymore. Now we are the manager and want to see if everything works in the background</t>
+  </si>
+  <si>
+    <t>The User should be in the Login Menu chosen from the Main Menu</t>
+  </si>
+  <si>
+    <t>1) Enter Email: [manager]
+2) Enter Password: [king]
+3) Press Enter</t>
+  </si>
+  <si>
+    <t>The User should now be in a overview window for the manager. There should be a Data table for orders and beneath it 3 Options to choose from.</t>
+  </si>
+  <si>
+    <t>UI014-N</t>
+  </si>
+  <si>
+    <t>We have the options as managment to either move the time forward, delete all open orders or return to the main menu. And the Manager should only be allowed to input one of the three options.</t>
+  </si>
+  <si>
+    <t>The User must be logged in as the manager. (Described in UI013)</t>
+  </si>
+  <si>
+    <t>Input: - [] ; [   ]
+- words or characters
+- negative numbers
+- positive numbers except 1-3</t>
+  </si>
+  <si>
+    <t>UI015</t>
+  </si>
+  <si>
+    <t>UI016</t>
+  </si>
+  <si>
+    <t>UI017</t>
+  </si>
+  <si>
+    <t>As the Manager we want to move the time forward to see if the orders are worked correctly and the system works</t>
+  </si>
+  <si>
+    <t>As the Manager we want to delete all closed orders so our drivers are free again and our overview gets emptier</t>
+  </si>
+  <si>
+    <t>As the Manager we ware finished with our work and want to Return / LogOut of the Manager Menu</t>
+  </si>
+  <si>
+    <t>1) Enter: [1]
+2) Press Enter</t>
+  </si>
+  <si>
+    <t>The Overview should reload and prep. Time, and Ship. Time should be decreased and some orders should have their statuses changed to Delivery. The User now has the possibility to choose again one of the menu points</t>
+  </si>
+  <si>
+    <t>1) Press: [2] 
+2) Press Enter</t>
+  </si>
+  <si>
+    <t>The User must be logged in as the manager. (Described in UI013). Ths User should repeat UI015 until at least one of the orders gets the status closed</t>
+  </si>
+  <si>
+    <t>The Overview should reload and every Order that had the status Closed should be removed from the overview. The User now has the possibility to choose again one of the menu points</t>
+  </si>
+  <si>
+    <t>1) Press: [3]
+2) Press Enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The User will be send to the Main menu from where he could LogIn again or register a new account. </t>
   </si>
 </sst>
 </file>
@@ -507,7 +1266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +1282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,7 +1319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,6 +1333,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,15 +1362,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1849755</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>426721</xdr:rowOff>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4402834</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>2952751</xdr:rowOff>
+      <xdr:colOff>2949319</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2724151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -621,8 +1392,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13279755" y="15142846"/>
-          <a:ext cx="2553079" cy="2526030"/>
+          <a:off x="11820525" y="14649451"/>
+          <a:ext cx="2558794" cy="2533650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -897,10 +1668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:I238"/>
+  <dimension ref="B2:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,56 +1687,42 @@
     <col min="9" max="9" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1" t="s">
+    <row r="2" spans="2:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -973,501 +1730,581 @@
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="2:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G11" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G13" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G15" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
+    <row r="16" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
       <c r="C16" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="G19" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
+    <row r="20" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="G21" s="2" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:9" ht="240.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+    <row r="27" spans="2:9" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="5"/>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
@@ -1950,52 +2787,59 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" s="4"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B81" s="3"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" s="4"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" s="4"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" s="4"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" s="4"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" s="4"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" s="4"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" s="4"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" s="4"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" s="4"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" s="4"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" s="4"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" s="4"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" s="4"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" s="4"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" s="4"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">
@@ -2424,7 +3268,13 @@
     <row r="238" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B238" s="4"/>
     </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B239" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:H2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>